<commit_message>
archivos de primer análisis
</commit_message>
<xml_diff>
--- a/analiticosxlsx/148.xlsx
+++ b/analiticosxlsx/148.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11017"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josemora/Documents/Github/Scrapers/Presupuesto 2023/analiticosxlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6259C278-C43D-C34B-A7A9-AC85DE7CCCDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBBB766-6483-E64E-B227-B644A6BF0380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-2160" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-1660" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2911,16 +2911,16 @@
       <c r="M50" s="24"/>
     </row>
     <row r="51" spans="1:13" ht="85" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="1"/>
+      <c r="A51" s="46" t="s">
+        <v>53</v>
+      </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="41"/>
       <c r="E51" s="41"/>
       <c r="F51" s="41"/>
       <c r="G51" s="41"/>
-      <c r="H51" s="46" t="s">
-        <v>53</v>
-      </c>
+      <c r="H51" s="46"/>
       <c r="I51" s="24"/>
       <c r="J51" s="24"/>
       <c r="K51" s="24"/>

</xml_diff>